<commit_message>
feat(market-data): add fallback mechanisms and instrument discovery
- Implement fallback LTP retrieval from instruments data when API fails
- Add instrument discovery to fetch eligible NSE/BSE equities
- Improve error handling and add alerts for data fetch failures
- Cache instrument universe to avoid repeated downloads
</commit_message>
<xml_diff>
--- a/transaction_log.xlsx
+++ b/transaction_log.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transactions'!$A$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transactions'!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -510,130 +510,8 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-12-31</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>09:20:00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>09:20:00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>TCS</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NSE:TCS</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>3755</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>febb9373-8f42-462a-be07-a38848adf7fe</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>FILLED</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>52W Breakout</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Strategy trigger: cross 52W boundary</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-12-31</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09:20:00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>09:20:00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>TCS</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>NSE:TCS</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>3793</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1581094e-0850-44f0-b674-b5d56cc770d0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>FILLED</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>52W Breakout</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Profit target hit</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M3"/>
+  <autoFilter ref="A1:M1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -671,7 +549,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -681,7 +559,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -691,7 +569,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>